<commit_message>
exploratory data analysis profiling and annex percentile
</commit_message>
<xml_diff>
--- a/exploratory_data_analysis/percentile_examples.xlsx
+++ b/exploratory_data_analysis/percentile_examples.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="38400" windowHeight="20180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>original variable</t>
   </si>
@@ -52,12 +52,18 @@
   <si>
     <t>Step 4</t>
   </si>
+  <si>
+    <t>How to calculate percentiles?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;ARS&quot;#,##0.00_);[Red]\(&quot;ARS&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,6 +135,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <i/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -200,6 +212,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -319,7 +333,7 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
-            <a:t>Case 1</a:t>
+            <a:t>Case 1:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -329,7 +343,7 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
-            <a:t>What is</a:t>
+            <a:t>Which is</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
@@ -354,7 +368,7 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
-            <a:t>Highest value for the 1st 50% of the ordered variable.</a:t>
+            <a:t>The highest value for the 1st 50% of the ordered variable.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -470,12 +484,12 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
+      <xdr:colOff>279400</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>292100</xdr:rowOff>
     </xdr:to>
@@ -486,8 +500,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6985000" y="5740400"/>
-          <a:ext cx="3060700" cy="1917700"/>
+          <a:off x="6985000" y="5308600"/>
+          <a:ext cx="3098800" cy="2349500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -540,8 +554,15 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
-            <a:t> the percentile 90th?</a:t>
-          </a:r>
+            <a:t> the percentile 90th? (or what is the value at 90th position?)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
+            <a:latin typeface="Times New Roman" charset="0"/>
+            <a:ea typeface="Times New Roman" charset="0"/>
+            <a:cs typeface="Times New Roman" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -550,7 +571,7 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
-            <a:t>It cannot be computed directly, we need to interpolate between the 83 and 92th percentile.</a:t>
+            <a:t>It cannot be computed directly, we need to interpolate between the 83th and 92nd percentile.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -852,11 +873,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
+      <xdr:colOff>330200</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>279400</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6007100" cy="1419619"/>
+    <xdr:ext cx="6007100" cy="2215991"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="20" name="TextBox 19"/>
@@ -864,8 +885,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4025900" y="8255000"/>
-          <a:ext cx="6007100" cy="1419619"/>
+          <a:off x="4203700" y="8051800"/>
+          <a:ext cx="6007100" cy="2215991"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -914,7 +935,62 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
-            <a:t>: R default </a:t>
+            <a:t>: The results may vary according to the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:rPr>
+            <a:t>interpolation</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:rPr>
+            <a:t> method</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0">
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:rPr>
+            <a:t>. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:rPr>
+            <a:t>There are many of them.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1800">
+            <a:latin typeface="Times New Roman" charset="0"/>
+            <a:ea typeface="Times New Roman" charset="0"/>
+            <a:cs typeface="Times New Roman" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:rPr>
+            <a:t>In </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" b="1">
@@ -922,6 +998,22 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
+            <a:t>R</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800">
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:rPr>
+            <a:t> the default </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" b="1">
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:rPr>
             <a:t>quantile</a:t>
           </a:r>
           <a:r>
@@ -930,7 +1022,7 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
-            <a:t> function uses an interpolation method.</a:t>
+            <a:t> function </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" baseline="0">
@@ -938,18 +1030,23 @@
               <a:ea typeface="Times New Roman" charset="0"/>
               <a:cs typeface="Times New Roman" charset="0"/>
             </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" baseline="0">
-              <a:latin typeface="Times New Roman" charset="0"/>
-              <a:ea typeface="Times New Roman" charset="0"/>
-              <a:cs typeface="Times New Roman" charset="0"/>
-            </a:rPr>
-            <a:t>Exact answers (in default type) are 54.5 and 130.5 for cases 1 and 2 respectevly. </a:t>
-          </a:r>
+            <a:t>retrieves the values 54.5 and 130.5 for cases 1 and 2 respectively. </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" i="1" baseline="0">
+              <a:latin typeface="Times New Roman" charset="0"/>
+              <a:ea typeface="Times New Roman" charset="0"/>
+              <a:cs typeface="Times New Roman" charset="0"/>
+            </a:rPr>
+            <a:t>In Microsoft Excel these values are slightly different.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1800" i="1" baseline="0">
+            <a:latin typeface="Times New Roman" charset="0"/>
+            <a:ea typeface="Times New Roman" charset="0"/>
+            <a:cs typeface="Times New Roman" charset="0"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -1093,6 +1190,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>56696</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>113393</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>272143</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>124732</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="884464" y="2267857"/>
+          <a:ext cx="9184822" cy="11339"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1363,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1477,9 +1618,11 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="25" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+      <c r="B10" s="21" t="s">
+        <v>9</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1495,7 +1638,6 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1755,7 +1897,7 @@
       <c r="K21" s="15"/>
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
+      <c r="N21" s="20"/>
     </row>
     <row r="22" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>

</xml_diff>

<commit_message>
main chang3s on high card var for pred mod (incomplete)
</commit_message>
<xml_diff>
--- a/exploratory_data_analysis/percentile_examples.xlsx
+++ b/exploratory_data_analysis/percentile_examples.xlsx
@@ -1504,13 +1504,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A10" zoomScale="116" zoomScaleNormal="116" zoomScalePageLayoutView="116" workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="7" width="10" customWidth="1"/>
+    <col min="2" max="3" width="10" customWidth="1"/>
+    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>